<commit_message>
- More details are given in Instructions.docx, including clarification on py2exe compilation
- Minor modifications to Service and Clinical applications
</commit_message>
<xml_diff>
--- a/iCOMCAT_CalibrationSequences.xlsx
+++ b/iCOMCAT_CalibrationSequences.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="34">
   <si>
     <t>6 MV</t>
   </si>
@@ -113,12 +113,18 @@
   <si>
     <t>CC</t>
   </si>
+  <si>
+    <t>We recommand to set Beam MU = 300</t>
+  </si>
+  <si>
+    <t>We recommand to set Beam MU = 1000</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,16 +132,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -143,11 +161,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -156,8 +190,13 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Entrée" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -457,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G181"/>
+  <dimension ref="A1:L181"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,7 +508,7 @@
     <col min="2" max="7" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -492,7 +531,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -515,7 +554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -537,8 +576,13 @@
       <c r="G3" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -561,7 +605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -584,17 +628,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -617,7 +661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -640,7 +684,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -663,7 +707,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -686,7 +730,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
@@ -709,7 +753,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>16</v>
       </c>
@@ -732,12 +776,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>18</v>
       </c>
@@ -760,7 +804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>19</v>
       </c>
@@ -4495,19 +4539,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C181"/>
+  <dimension ref="A1:H181"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.5703125" style="2" customWidth="1"/>
     <col min="2" max="3" width="11.42578125" style="1"/>
+    <col min="8" max="8" width="12.5703125" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -4518,12 +4564,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -4533,8 +4579,13 @@
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -4545,7 +4596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -4556,17 +4607,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -4577,12 +4628,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -4593,7 +4644,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -4604,7 +4655,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
@@ -4615,7 +4666,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>16</v>
       </c>
@@ -4626,12 +4677,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>18</v>
       </c>
@@ -4642,7 +4693,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>19</v>
       </c>
@@ -6445,19 +6496,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C181"/>
+  <dimension ref="A1:H181"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.5703125" style="2" customWidth="1"/>
     <col min="2" max="3" width="11.42578125" style="1"/>
+    <col min="8" max="8" width="12.28515625" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -6468,12 +6521,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -6483,8 +6536,13 @@
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -6495,7 +6553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -6506,17 +6564,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -6527,12 +6585,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -6543,7 +6601,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -6554,7 +6612,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
@@ -6565,7 +6623,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>16</v>
       </c>
@@ -6576,12 +6634,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>18</v>
       </c>
@@ -6592,7 +6650,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>19</v>
       </c>

</xml_diff>